<commit_message>
Updated win_prob calcs and inluded custom metrics
</commit_message>
<xml_diff>
--- a/matchups.xlsx
+++ b/matchups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/austinlanglinais/Documents/march-madness/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C036BB5F-05CD-5046-B2AF-061C06BE4FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9789A4F-D775-394D-9435-A101E89C89DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17180" xr2:uid="{FE2FDFD0-57E3-E244-92E6-5F30D74A8644}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="68">
   <si>
     <t>team_1</t>
   </si>
@@ -263,7 +263,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -271,12 +271,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -611,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DFDEEEF-0A97-9B46-BC23-F8DABCB4FDD9}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="A50" sqref="A50:B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1071,18 +1081,146 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="33" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
         <v>2</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
         <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>60</v>
+      </c>
+      <c r="B48" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Both an art and a science a.k.a the Memphis problem
</commit_message>
<xml_diff>
--- a/matchups.xlsx
+++ b/matchups.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/austinlanglinais/Documents/march-madness/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9789A4F-D775-394D-9435-A101E89C89DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4EC84AE-AAFF-624E-9203-183A0B5A52CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17180" xr2:uid="{FE2FDFD0-57E3-E244-92E6-5F30D74A8644}"/>
+    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="17180" xr2:uid="{FE2FDFD0-57E3-E244-92E6-5F30D74A8644}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="68">
   <si>
     <t>team_1</t>
   </si>
@@ -284,9 +284,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DFDEEEF-0A97-9B46-BC23-F8DABCB4FDD9}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:B51"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -633,17 +634,17 @@
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1102,6 +1103,12 @@
       <c r="B34" t="s">
         <v>6</v>
       </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>8</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
@@ -1110,13 +1117,25 @@
       <c r="B35" t="s">
         <v>10</v>
       </c>
+      <c r="C35">
+        <v>5</v>
+      </c>
+      <c r="D35">
+        <v>4</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B36" t="s">
         <v>14</v>
+      </c>
+      <c r="C36">
+        <v>11</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1126,6 +1145,12 @@
       <c r="B37" t="s">
         <v>18</v>
       </c>
+      <c r="C37">
+        <v>7</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
@@ -1134,13 +1159,25 @@
       <c r="B38" t="s">
         <v>22</v>
       </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>8</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>24</v>
       </c>
       <c r="B39" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="C39">
+        <v>5</v>
+      </c>
+      <c r="D39">
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1150,6 +1187,12 @@
       <c r="B40" t="s">
         <v>30</v>
       </c>
+      <c r="C40">
+        <v>11</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
@@ -1158,6 +1201,12 @@
       <c r="B41" t="s">
         <v>34</v>
       </c>
+      <c r="C41">
+        <v>7</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
@@ -1166,6 +1215,12 @@
       <c r="B42" t="s">
         <v>38</v>
       </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>8</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -1174,6 +1229,12 @@
       <c r="B43" t="s">
         <v>43</v>
       </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+      <c r="D43">
+        <v>13</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
@@ -1182,6 +1243,12 @@
       <c r="B44" t="s">
         <v>46</v>
       </c>
+      <c r="C44">
+        <v>6</v>
+      </c>
+      <c r="D44">
+        <v>3</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
@@ -1190,13 +1257,25 @@
       <c r="B45" t="s">
         <v>50</v>
       </c>
+      <c r="C45">
+        <v>7</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1204,7 +1283,13 @@
         <v>56</v>
       </c>
       <c r="B47" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1214,13 +1299,235 @@
       <c r="B48" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="C48">
+        <v>11</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="1" t="s">
         <v>65</v>
+      </c>
+      <c r="C49" s="1">
+        <v>7</v>
+      </c>
+      <c r="D49" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>13</v>
+      </c>
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51">
+        <v>11</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" t="s">
+        <v>24</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>29</v>
+      </c>
+      <c r="B53" t="s">
+        <v>34</v>
+      </c>
+      <c r="C53">
+        <v>11</v>
+      </c>
+      <c r="D53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>36</v>
+      </c>
+      <c r="B54" t="s">
+        <v>40</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55">
+        <v>6</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56" t="s">
+        <v>56</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C57" s="1">
+        <v>3</v>
+      </c>
+      <c r="D57" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>4</v>
+      </c>
+      <c r="B58" t="s">
+        <v>18</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>24</v>
+      </c>
+      <c r="B59" t="s">
+        <v>34</v>
+      </c>
+      <c r="C59">
+        <v>5</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>36</v>
+      </c>
+      <c r="B60" t="s">
+        <v>44</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61" s="1">
+        <v>1</v>
+      </c>
+      <c r="D61" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" t="s">
+        <v>34</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C63" s="1">
+        <v>1</v>
+      </c>
+      <c r="D63" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C64" s="2">
+        <v>5</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final tweaing + viz tool
</commit_message>
<xml_diff>
--- a/matchups.xlsx
+++ b/matchups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/austinlanglinais/Documents/march-madness/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4EC84AE-AAFF-624E-9203-183A0B5A52CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15B6165-B7EE-B440-9F84-61359378310B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="17180" xr2:uid="{FE2FDFD0-57E3-E244-92E6-5F30D74A8644}"/>
   </bookViews>
@@ -284,10 +284,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DFDEEEF-0A97-9B46-BC23-F8DABCB4FDD9}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1415,7 +1414,7 @@
         <v>1</v>
       </c>
       <c r="D56">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1448,7 +1447,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B59" t="s">
         <v>34</v>
@@ -1493,13 +1492,13 @@
         <v>4</v>
       </c>
       <c r="B62" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
       <c r="D62">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1517,16 +1516,16 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B64" s="2" t="s">
+      <c r="A64" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64" t="s">
         <v>36</v>
       </c>
-      <c r="C64" s="2">
-        <v>5</v>
-      </c>
-      <c r="D64" s="2">
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
         <v>1</v>
       </c>
     </row>

</xml_diff>